<commit_message>
maj devis et factures
</commit_message>
<xml_diff>
--- a/devis/Devis_OpcaDefi_Forfait_florian_01_2017.xlsx
+++ b/devis/Devis_OpcaDefi_Forfait_florian_01_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Florian CHAUMEIL</t>
   </si>
@@ -116,98 +116,6 @@
     <t>€</t>
   </si>
   <si>
-    <t>et du module de synchro montante:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tests des chaines complètes de saisies</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Demande de prise plan </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Demande multi établissement </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Demande multi dispositif </t>
-    </r>
-  </si>
-  <si>
     <t>Total HT</t>
   </si>
   <si>
@@ -244,37 +152,52 @@
     <t>Tarif forfait jours TTC</t>
   </si>
   <si>
-    <t>-       Assistance aux tests fonctionnels  de pré-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Déploiement des api de synchro mcd-optiform</t>
-  </si>
-  <si>
-    <t>-       Résolution d'erreurs de saisie utilisateurs MCD</t>
-  </si>
-  <si>
-    <t>Préparation à la mise en production de l'EDI salarié</t>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>cotis</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>pas de différence entre le Hors Taxe (HT) et le Toutes Taxes Comprises (TTC). Vous ne collectez pas la TVA pour l'Etat, le montant de la prestation ne tient pas compte de la TVA. </t>
+  </si>
+  <si>
+    <t>-       Assistance aux tests fonctionnels  et recette</t>
   </si>
   <si>
     <t>-       Evolution des modules de synchronisation</t>
   </si>
   <si>
-    <t>-       Adaptation des vues nécessaires aux API v2</t>
-  </si>
-  <si>
-    <t>Tâches diverses</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>cotis</t>
-  </si>
-  <si>
-    <t>net</t>
-  </si>
-  <si>
-    <t>Vous ne faites pas de différence entre le Hors Taxe (HT) et le Toutes Taxes Comprises (TTC). Vous ne collectez pas la TVA pour l'Etat, votre prix de vente ne tient donc pas compte de la TVA. En revanche, lors de vos achats, vous payez la TVA à votre fournisseur (qui n'est pas auto-entrepreneur) mais vous ne pouvez pas la récupérer auprès de l'Etat. </t>
+    <t xml:space="preserve">       des api de synchro mcd-optiform et EDI Salarié</t>
+  </si>
+  <si>
+    <t>-       mise en place d'un processus (applicatif, API)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       automatisé de dépose de fichier EDI</t>
+  </si>
+  <si>
+    <t>Préparation et suivi de la mise en production de l'EDI</t>
+  </si>
+  <si>
+    <t>salarié et du module de synchro montante:</t>
+  </si>
+  <si>
+    <t>-       Assistance technique à la mise en prod EDI salarié</t>
+  </si>
+  <si>
+    <t>Automatisation de la dépose EDI Salarié:</t>
+  </si>
+  <si>
+    <t>Etudes préliminaires EDI PEC:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-       Analyse du processus actuel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-       rédaction d'une doc technico-fonctionnelle </t>
   </si>
 </sst>
 </file>
@@ -287,7 +210,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-407]"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,59 +320,41 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -478,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -595,21 +500,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -654,9 +544,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -700,7 +590,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -708,56 +597,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="14" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H14:M26"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,9 +986,9 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="G1" s="49" t="str">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="G1" s="43" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("Devis n° ",B6)</f>
         <v>Devis n° 2</v>
       </c>
@@ -1118,7 +1009,7 @@
       </c>
       <c r="B5" s="5">
         <f ca="1">TODAY()</f>
-        <v>42732</v>
+        <v>42734</v>
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="9" t="s">
@@ -1165,7 +1056,7 @@
       </c>
       <c r="C8" s="5"/>
       <c r="E8" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1212,7 +1103,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5">
         <f>DATE(2016,12,19)+0</f>
@@ -1227,7 +1118,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5">
         <f>DATE(2016,12,30)+0</f>
@@ -1235,7 +1126,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1244,22 +1135,22 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="38">
-        <f>SUM(E25:E37)</f>
-        <v>4.5</v>
+      <c r="B14" s="36">
+        <f>SUM(E24:E36)</f>
+        <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4">
         <v>312</v>
@@ -1273,7 +1164,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="J15" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K15" s="2">
         <v>3120</v>
@@ -1281,268 +1172,282 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J16" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K16" s="2">
         <v>720</v>
       </c>
-      <c r="L16" s="66">
+      <c r="L16" s="57">
         <f>K16/K15</f>
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" s="2">
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="2">
         <f>K15-K16</f>
         <v>2400</v>
       </c>
     </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>20</v>
+      <c r="A19" s="18" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>21</v>
+      <c r="A20" s="17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="65"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="64">
+        <v>42748</v>
+      </c>
+      <c r="E24" s="66"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="32">
+        <f>SUM(E24:E30)*B15</f>
+        <v>1248</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>50</v>
+      <c r="A25" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="B25" s="28"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60">
-        <v>42741</v>
-      </c>
-      <c r="E25" s="56"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="28"/>
-      <c r="G25" s="33">
-        <f>SUM(E25:E30)*B15</f>
-        <v>1248</v>
-      </c>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
+      <c r="A26" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="61">
+        <v>1</v>
+      </c>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="61">
+        <v>1</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="56">
-        <v>2</v>
-      </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="61">
+        <v>1</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="56">
-        <v>2</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="61">
+        <v>1</v>
+      </c>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="48">
-        <v>42734</v>
-      </c>
-      <c r="E31" s="56"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="34">
-        <f>SUM(E31:E35)*$B$15</f>
-        <v>0</v>
+      <c r="A30" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="33">
+        <f>SUM(E32:E33)*$B$15</f>
+        <v>1560</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="61">
+        <v>2</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="61">
+        <v>3</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="56">
+        <v>1</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="33">
+        <f>SUM(E34:E36)*$B$15</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="34">
+        <f>SUM(G24:G36)</f>
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="15"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="37"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="49">
+        <f>G37+G39</f>
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="35" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="34">
-        <f>SUM(E36:E37)*$B$15</f>
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="57">
-        <v>0.5</v>
-      </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G38" s="36">
-        <f>SUM(G25:G37)</f>
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="15"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="G42" s="55">
-        <f>G38+G40</f>
-        <v>1404</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="37" t="s">
-        <v>38</v>
-      </c>
+      <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D45" s="8"/>
@@ -1556,76 +1461,64 @@
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20" t="s">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
         <v>1</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
-        <v>2</v>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
-      <c r="D52" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="D52" s="23"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
getting the ball rollin'
</commit_message>
<xml_diff>
--- a/devis/Devis_OpcaDefi_Forfait_florian_01_2017.xlsx
+++ b/devis/Devis_OpcaDefi_Forfait_florian_01_2017.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Florian CHAUMEIL</t>
   </si>
@@ -165,33 +165,6 @@
     <t>pas de différence entre le Hors Taxe (HT) et le Toutes Taxes Comprises (TTC). Vous ne collectez pas la TVA pour l'Etat, le montant de la prestation ne tient pas compte de la TVA. </t>
   </si>
   <si>
-    <t>-       Assistance aux tests fonctionnels  et recette</t>
-  </si>
-  <si>
-    <t>-       Evolution des modules de synchronisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       des api de synchro mcd-optiform et EDI Salarié</t>
-  </si>
-  <si>
-    <t>-       mise en place d'un processus (applicatif, API)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       automatisé de dépose de fichier EDI</t>
-  </si>
-  <si>
-    <t>Préparation et suivi de la mise en production de l'EDI</t>
-  </si>
-  <si>
-    <t>salarié et du module de synchro montante:</t>
-  </si>
-  <si>
-    <t>-       Assistance technique à la mise en prod EDI salarié</t>
-  </si>
-  <si>
-    <t>Automatisation de la dépose EDI Salarié:</t>
-  </si>
-  <si>
     <t>Etudes préliminaires EDI PEC:</t>
   </si>
   <si>
@@ -201,7 +174,43 @@
     <t xml:space="preserve">-       rédaction d'une doc technico-fonctionnelle </t>
   </si>
   <si>
-    <t>-       Maintenance vues et api en relation avec Globalys</t>
+    <t>Référence</t>
+  </si>
+  <si>
+    <t>opcadefi012017/d2</t>
+  </si>
+  <si>
+    <t>Devis</t>
+  </si>
+  <si>
+    <t>Adaptation processus existants:</t>
+  </si>
+  <si>
+    <t>Test API v2</t>
+  </si>
+  <si>
+    <t>-      Lancement des api hauts volumes</t>
+  </si>
+  <si>
+    <t>-       modules de synchro (refacto,script deploiement</t>
+  </si>
+  <si>
+    <t>unification fichiers config)</t>
+  </si>
+  <si>
+    <t>-       Ajout rct&amp;prod table ID pec + code de remplissage</t>
+  </si>
+  <si>
+    <t>diagnostique + fix erreur saisie et PS</t>
+  </si>
+  <si>
+    <t>-      test chaine complete (dpec, cpro)</t>
+  </si>
+  <si>
+    <t>-       api (unite stagiaire, cout, option group fin)</t>
+  </si>
+  <si>
+    <t>-      Suivi debug en relation avec Globalys</t>
   </si>
 </sst>
 </file>
@@ -214,7 +223,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-407]"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +367,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -501,19 +522,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -539,6 +547,21 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -552,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -594,7 +617,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -615,7 +637,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -630,40 +651,60 @@
     <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,16 +1042,23 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="G1" s="42" t="str">
-        <f xml:space="preserve"> _xlfn.CONCAT("Devis n° ",B6)</f>
-        <v>Devis n° 2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="73"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="72"/>
+      <c r="G2" s="71" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1024,7 +1072,7 @@
       </c>
       <c r="B5" s="5">
         <f ca="1">TODAY()</f>
-        <v>42737</v>
+        <v>42773</v>
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="9" t="s">
@@ -1037,8 +1085,9 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
+      <c r="B6" s="4" t="str">
+        <f>G2</f>
+        <v>opcadefi012017/d2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="11" t="s">
@@ -1121,8 +1170,8 @@
         <v>36</v>
       </c>
       <c r="B12" s="5">
-        <f>DATE(2017,1,3)+0</f>
-        <v>42738</v>
+        <f>DATE(2017,1,16)+0</f>
+        <v>42751</v>
       </c>
       <c r="C12" s="5"/>
       <c r="E12" s="11" t="s">
@@ -1137,7 +1186,7 @@
       </c>
       <c r="B13" s="5">
         <f>D24</f>
-        <v>42748</v>
+        <v>42766</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="11" t="s">
@@ -1150,9 +1199,9 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="35">
         <f>SUM(E24:E33)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>12</v>
@@ -1178,339 +1227,332 @@
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="59" t="s">
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="38" t="s">
+      <c r="E23" s="58"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="37" t="s">
         <v>38</v>
       </c>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="63">
-        <v>42748</v>
-      </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="32">
-        <f>SUM(E24:E30)*B15</f>
-        <v>2496</v>
-      </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
+      <c r="A24" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="76">
+        <v>42766</v>
+      </c>
+      <c r="E24" s="59"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="31">
+        <f>SUM(E24:E27)*B15</f>
+        <v>1560</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="56">
+        <v>1</v>
+      </c>
+      <c r="F25" s="68"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="56">
+        <v>2</v>
+      </c>
+      <c r="F26" s="68"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="56">
+        <v>2</v>
+      </c>
+      <c r="F27" s="68"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="60"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="74">
+        <v>1</v>
+      </c>
+      <c r="F28" s="75"/>
+      <c r="G28" s="82">
+        <f>SUM(E28:E28)*$B$15</f>
+        <v>312</v>
+      </c>
+      <c r="H28" s="64"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="60">
+      <c r="B29" s="26"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="31">
+        <f>SUM(E29:E33)*$B$15</f>
+        <v>1560</v>
+      </c>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="47">
         <v>2</v>
       </c>
-      <c r="F26" s="75"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="60">
+      <c r="F30" s="68"/>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="47">
         <v>1</v>
       </c>
-      <c r="F27" s="75"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="60">
-        <v>2</v>
-      </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="67"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="60">
+      <c r="F31" s="68"/>
+      <c r="G31" s="31"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="47">
         <v>1</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="61">
-        <v>2</v>
-      </c>
-      <c r="F30" s="75"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="72"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="55">
+      <c r="F32" s="68"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="48">
         <v>1</v>
       </c>
-      <c r="F31" s="74"/>
-      <c r="G31" s="33">
-        <f>SUM(E31:E33)*$B$15</f>
-        <v>312</v>
-      </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="31"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="33">
         <f>SUM(G24:G33)</f>
-        <v>2808</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="43" t="s">
+      <c r="G35" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="44" t="s">
+      <c r="F36" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="45">
+      <c r="G36" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E37" s="15"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="37"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="47" t="s">
+      <c r="F38" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="G38" s="48">
+      <c r="G38" s="46">
         <f>G34+G36</f>
-        <v>2808</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="34" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1593,7 +1635,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D24:D33"/>
   </mergeCells>
   <pageMargins left="0.625" right="0.44791666666666669" top="0.48958333333333331" bottom="0.33088235294117646" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1681,7 +1723,7 @@
       <c r="E11" s="2">
         <v>720</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="53">
         <f>E11/E10</f>
         <v>0.23076923076923078</v>
       </c>
@@ -1795,44 +1837,44 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="33">
+      <c r="B23" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="32">
         <f>SUM(F24:F25)*$B$15</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="60">
+      <c r="B24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="56">
         <v>2</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="60">
+      <c r="B25" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="56">
         <v>3</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>

</xml_diff>